<commit_message>
Update Template Network Connection Tab calculation for disconnect
</commit_message>
<xml_diff>
--- a/SRUM_TEMPLATE.xlsx
+++ b/SRUM_TEMPLATE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\host\Documents\PythonProjects\srum\srum-dump\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\shared folders\E\Documents\PythonProjects\srum\srum-dump\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18285" windowHeight="6390" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18285" windowHeight="6390" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Network Usage" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Energy Usage" sheetId="6" r:id="rId6"/>
     <sheet name="Undocumented Windows 10 Table" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" iterate="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -209,9 +209,6 @@
     <t>ConnectStartTime</t>
   </si>
   <si>
-    <t>=H#ROW_NUM#+G#ROW_NUM#/86400</t>
-  </si>
-  <si>
     <t>SRUM Entry ID</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>{97C2CE28-A37B-4920-B1E9-8B76CD341EC5}</t>
+  </si>
+  <si>
+    <t>=H#ROW_NUM#+G#ROW_NUM#</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -774,7 +774,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -809,49 +809,49 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -895,49 +895,49 @@
         <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>80</v>
+      <c r="H4" s="4" t="s">
+        <v>65</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1023,22 +1023,22 @@
         <v>13</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>17</v>
@@ -1053,13 +1053,13 @@
         <v>5</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>58</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>6</v>
@@ -1075,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
@@ -66923,7 +66923,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>

</xml_diff>